<commit_message>
Inclusão da margem de despesas
</commit_message>
<xml_diff>
--- a/diagnostico_art_setimo_propag_new.xlsx
+++ b/diagnostico_art_setimo_propag_new.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -380,22 +380,32 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>variacao_2024_2023_corrigida</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>resultado_primario</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>condicao_I</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>condicao_II</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>condicao_III</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>margem_despesa</t>
         </is>
       </c>
     </row>
@@ -415,16 +425,22 @@
         <v>46132680103.83968</v>
       </c>
       <c r="E2">
+        <v>0.07217724455430408</v>
+      </c>
+      <c r="F2">
         <v>2519505074.18</v>
       </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
       <c r="G2" t="b">
         <v>0</v>
       </c>
       <c r="H2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0.09882407118801286</v>
       </c>
     </row>
     <row r="3">
@@ -443,16 +459,22 @@
         <v>42166540028.2124</v>
       </c>
       <c r="E3">
+        <v>0.05687339318765683</v>
+      </c>
+      <c r="F3">
         <v>2350124188.12</v>
       </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
       <c r="G3" t="b">
         <v>0</v>
       </c>
       <c r="H3" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0.08811137523135978</v>
       </c>
     </row>
     <row r="4">
@@ -471,16 +493,22 @@
         <v>20684300259.17596</v>
       </c>
       <c r="E4">
+        <v>0.007747811020725637</v>
+      </c>
+      <c r="F4">
         <v>314183267.4</v>
       </c>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
       <c r="G4" t="b">
         <v>0</v>
       </c>
       <c r="H4" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0.05372346771450795</v>
       </c>
     </row>
     <row r="5">
@@ -499,16 +527,22 @@
         <v>14074899183.29466</v>
       </c>
       <c r="E5">
+        <v>0.1099054456163597</v>
+      </c>
+      <c r="F5">
         <v>511881947.09</v>
       </c>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
       <c r="G5" t="b">
         <v>0</v>
       </c>
       <c r="H5" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0.1252338119314518</v>
       </c>
     </row>
     <row r="6">
@@ -527,16 +561,22 @@
         <v>24105422832.37936</v>
       </c>
       <c r="E6">
+        <v>-0.02474494835859653</v>
+      </c>
+      <c r="F6">
         <v>-816011689.04</v>
       </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
       <c r="G6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0.0483</v>
       </c>
     </row>
     <row r="7">
@@ -555,16 +595,22 @@
         <v>14548657872.4048</v>
       </c>
       <c r="E7">
+        <v>0.1412448032998892</v>
+      </c>
+      <c r="F7">
         <v>1668810600.37</v>
       </c>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
       <c r="G7" t="b">
         <v>0</v>
       </c>
       <c r="H7" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0.1471713623099225</v>
       </c>
     </row>
     <row r="8">
@@ -583,16 +629,22 @@
         <v>76299632094.53944</v>
       </c>
       <c r="E8">
+        <v>-0.070301201882641</v>
+      </c>
+      <c r="F8">
         <v>54645113.55</v>
       </c>
-      <c r="F8" t="b">
-        <v>1</v>
-      </c>
       <c r="G8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0.0483</v>
       </c>
     </row>
     <row r="9">
@@ -611,16 +663,22 @@
         <v>35637878828.10659</v>
       </c>
       <c r="E9">
+        <v>0.02754410892825732</v>
+      </c>
+      <c r="F9">
         <v>-1162719962.55</v>
       </c>
-      <c r="F9" t="b">
-        <v>0</v>
-      </c>
       <c r="G9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0.06207205446412866</v>
       </c>
     </row>
     <row r="10">
@@ -636,19 +694,25 @@
         <v>79898987775.5</v>
       </c>
       <c r="D10">
-        <v>79598557003.43983</v>
+        <v>79598557003.43984</v>
       </c>
       <c r="E10">
+        <v>0.003774324351723868</v>
+      </c>
+      <c r="F10">
         <v>2156932130.84</v>
       </c>
-      <c r="F10" t="b">
-        <v>0</v>
-      </c>
       <c r="G10" t="b">
         <v>0</v>
       </c>
       <c r="H10" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0.05094202704620671</v>
       </c>
     </row>
     <row r="11">
@@ -667,16 +731,22 @@
         <v>24517779585.84155</v>
       </c>
       <c r="E11">
+        <v>0.1041603739215926</v>
+      </c>
+      <c r="F11">
         <v>465138744.19</v>
       </c>
-      <c r="F11" t="b">
-        <v>0</v>
-      </c>
       <c r="G11" t="b">
         <v>0</v>
       </c>
       <c r="H11" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0.1212122617451148</v>
       </c>
     </row>
     <row r="12">
@@ -692,19 +762,25 @@
         <v>8398145478.81</v>
       </c>
       <c r="D12">
-        <v>7751748405.04845</v>
+        <v>7751748405.048451</v>
       </c>
       <c r="E12">
+        <v>0.08338726181316369</v>
+      </c>
+      <c r="F12">
         <v>224862163.24</v>
       </c>
-      <c r="F12" t="b">
-        <v>0</v>
-      </c>
       <c r="G12" t="b">
         <v>0</v>
       </c>
       <c r="H12" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0.1066710832692146</v>
       </c>
     </row>
     <row r="13">
@@ -723,16 +799,22 @@
         <v>15600493570.36323</v>
       </c>
       <c r="E13">
+        <v>0.05872842322164051</v>
+      </c>
+      <c r="F13">
         <v>112212752.54</v>
       </c>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
       <c r="G13" t="b">
         <v>0</v>
       </c>
       <c r="H13" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0.08940989625514836</v>
       </c>
     </row>
     <row r="14">
@@ -751,16 +833,22 @@
         <v>95611503950.16649</v>
       </c>
       <c r="E14">
+        <v>-0.008622525589663144</v>
+      </c>
+      <c r="F14">
         <v>1071629655.61</v>
       </c>
-      <c r="F14" t="b">
-        <v>1</v>
-      </c>
       <c r="G14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0.0483</v>
       </c>
     </row>
     <row r="15">
@@ -779,16 +867,22 @@
         <v>329355602961.1492</v>
       </c>
       <c r="E15">
+        <v>0.04799685304602352</v>
+      </c>
+      <c r="F15">
         <v>12941505872.87</v>
       </c>
-      <c r="F15" t="b">
-        <v>0</v>
-      </c>
       <c r="G15" t="b">
         <v>0</v>
       </c>
       <c r="H15" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0.08189779713221647</v>
       </c>
     </row>
     <row r="16">
@@ -807,16 +901,22 @@
         <v>112481103541.5773</v>
       </c>
       <c r="E16">
+        <v>0.06807493135104581</v>
+      </c>
+      <c r="F16">
         <v>4536879197.55</v>
       </c>
-      <c r="F16" t="b">
-        <v>0</v>
-      </c>
       <c r="G16" t="b">
         <v>0</v>
       </c>
       <c r="H16" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0.09595245194573207</v>
       </c>
     </row>
     <row r="17">
@@ -835,16 +935,22 @@
         <v>18463452259.67506</v>
       </c>
       <c r="E17">
+        <v>0.07650302863077885</v>
+      </c>
+      <c r="F17">
         <v>23103237.4</v>
       </c>
-      <c r="F17" t="b">
-        <v>0</v>
-      </c>
       <c r="G17" t="b">
         <v>0</v>
       </c>
       <c r="H17" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0.1018521200415452</v>
       </c>
     </row>
     <row r="18">
@@ -863,16 +969,22 @@
         <v>66631789838.73751</v>
       </c>
       <c r="E18">
+        <v>0.04214346369921396</v>
+      </c>
+      <c r="F18">
         <v>-816732338.65</v>
       </c>
-      <c r="F18" t="b">
-        <v>0</v>
-      </c>
       <c r="G18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0.06937173184960699</v>
       </c>
     </row>
     <row r="19">
@@ -891,16 +1003,22 @@
         <v>26196028260.1499</v>
       </c>
       <c r="E19">
+        <v>0.2171278419413167</v>
+      </c>
+      <c r="F19">
         <v>3361964541.35</v>
       </c>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
       <c r="G19" t="b">
         <v>0</v>
       </c>
       <c r="H19" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>0.2002894893589217</v>
       </c>
     </row>
     <row r="20">
@@ -919,16 +1037,22 @@
         <v>50373356805.65094</v>
       </c>
       <c r="E20">
+        <v>-0.0587844644861697</v>
+      </c>
+      <c r="F20">
         <v>1305075783.32</v>
       </c>
-      <c r="F20" t="b">
-        <v>1</v>
-      </c>
       <c r="G20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0.0483</v>
       </c>
     </row>
     <row r="21">
@@ -947,16 +1071,22 @@
         <v>16234182507.38882</v>
       </c>
       <c r="E21">
+        <v>0.120880003691471</v>
+      </c>
+      <c r="F21">
         <v>399317766.75</v>
       </c>
-      <c r="F21" t="b">
-        <v>0</v>
-      </c>
       <c r="G21" t="b">
         <v>0</v>
       </c>
       <c r="H21" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>0.1329160025840297</v>
       </c>
     </row>
     <row r="22">
@@ -975,16 +1105,22 @@
         <v>10443002270.10554</v>
       </c>
       <c r="E22">
+        <v>0.1185231531470266</v>
+      </c>
+      <c r="F22">
         <v>669889295.9</v>
       </c>
-      <c r="F22" t="b">
-        <v>0</v>
-      </c>
       <c r="G22" t="b">
         <v>0</v>
       </c>
       <c r="H22" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>0.1312662072029186</v>
       </c>
     </row>
     <row r="23">
@@ -1003,16 +1139,22 @@
         <v>18486027609.51009</v>
       </c>
       <c r="E23">
+        <v>0.06235166936010317</v>
+      </c>
+      <c r="F23">
         <v>-1733005722.17</v>
       </c>
-      <c r="F23" t="b">
-        <v>0</v>
-      </c>
       <c r="G23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I23" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0.07947583468005159</v>
       </c>
     </row>
     <row r="24">
@@ -1031,16 +1173,22 @@
         <v>29802085746.79517</v>
       </c>
       <c r="E24">
+        <v>0.1009291003082993</v>
+      </c>
+      <c r="F24">
         <v>404575321.53</v>
       </c>
-      <c r="F24" t="b">
-        <v>0</v>
-      </c>
       <c r="G24" t="b">
         <v>0</v>
       </c>
       <c r="H24" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>0.1189503702158095</v>
       </c>
     </row>
     <row r="25">
@@ -1059,16 +1207,22 @@
         <v>35819310586.55398</v>
       </c>
       <c r="E25">
+        <v>0.05282282983040654</v>
+      </c>
+      <c r="F25">
         <v>-644665912.25</v>
       </c>
-      <c r="F25" t="b">
-        <v>0</v>
-      </c>
       <c r="G25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0.07471141491520328</v>
       </c>
     </row>
     <row r="26">
@@ -1087,16 +1241,22 @@
         <v>8783153768.204992</v>
       </c>
       <c r="E26">
+        <v>0.116571484716731</v>
+      </c>
+      <c r="F26">
         <v>444629422.93</v>
       </c>
-      <c r="F26" t="b">
-        <v>0</v>
-      </c>
       <c r="G26" t="b">
         <v>0</v>
       </c>
       <c r="H26" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>0.1299000393017117</v>
       </c>
     </row>
     <row r="27">
@@ -1112,19 +1272,25 @@
         <v>40056003880.13</v>
       </c>
       <c r="D27">
-        <v>36466069939.88293</v>
+        <v>36466069939.88294</v>
       </c>
       <c r="E27">
+        <v>0.09844586889032292</v>
+      </c>
+      <c r="F27">
         <v>417230647.02</v>
       </c>
-      <c r="F27" t="b">
-        <v>0</v>
-      </c>
       <c r="G27" t="b">
         <v>0</v>
       </c>
       <c r="H27" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>0.117212108223226</v>
       </c>
     </row>
     <row r="28">
@@ -1143,16 +1309,22 @@
         <v>42289180161.18084</v>
       </c>
       <c r="E28">
+        <v>0.07476567041636573</v>
+      </c>
+      <c r="F28">
         <v>-1890220391.49</v>
       </c>
-      <c r="F28" t="b">
-        <v>0</v>
-      </c>
       <c r="G28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0.08568283520818287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>